<commit_message>
[Fix Bug] Fix some bugs of ConfigEditor. [Add Feature] Add ConfigManager.
</commit_message>
<xml_diff>
--- a/Files/Config/TestData.xlsx
+++ b/Files/Config/TestData.xlsx
@@ -27,7 +27,7 @@
     <t>value</t>
   </si>
   <si>
-    <t>int</t>
+    <t>long</t>
   </si>
   <si>
     <t>string</t>
@@ -60,9 +60,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="1">
     <font>

</xml_diff>

<commit_message>
[Add Feature]Add support of bool value parse in ConfigEditor.
</commit_message>
<xml_diff>
--- a/Files/Config/TestData.xlsx
+++ b/Files/Config/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28710" windowHeight="13050"/>
+    <workbookView windowWidth="28695" windowHeight="13125"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
   <si>
     <t>id</t>
   </si>
@@ -27,6 +27,9 @@
     <t>value</t>
   </si>
   <si>
+    <t>testBool</t>
+  </si>
+  <si>
     <t>long</t>
   </si>
   <si>
@@ -36,6 +39,9 @@
     <t>float</t>
   </si>
   <si>
+    <t>bool</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
@@ -45,13 +51,13 @@
     <t>数值</t>
   </si>
   <si>
+    <t>测试布尔值</t>
+  </si>
+  <si>
     <t>test1</t>
   </si>
   <si>
     <t>测试1</t>
-  </si>
-  <si>
-    <t>test3</t>
   </si>
 </sst>
 </file>
@@ -59,27 +65,364 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -87,24 +430,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -113,13 +683,56 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -170,71 +783,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
         <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
         <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
         <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
         <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,19 +1066,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
     <col min="2" max="2" width="16.875" customWidth="1"/>
     <col min="3" max="3" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,58 +1088,71 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>0.13</v>
       </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>3.1415926</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
+      <c r="B6"/>
       <c r="C6">
         <v>1234</v>
       </c>

</xml_diff>

<commit_message>
[Add Feature]Add support of byte and sbyte value parse in ConfigEditor.
</commit_message>
<xml_diff>
--- a/Files/Config/TestData.xlsx
+++ b/Files/Config/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
   <si>
     <t>id</t>
   </si>
@@ -30,6 +30,12 @@
     <t>testBool</t>
   </si>
   <si>
+    <t>testByte</t>
+  </si>
+  <si>
+    <t>testSByte</t>
+  </si>
+  <si>
     <t>long</t>
   </si>
   <si>
@@ -42,6 +48,12 @@
     <t>bool</t>
   </si>
   <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>sbyte</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
@@ -52,6 +64,12 @@
   </si>
   <si>
     <t>测试布尔值</t>
+  </si>
+  <si>
+    <t>测试byte</t>
+  </si>
+  <si>
+    <t>测试sbyte</t>
   </si>
   <si>
     <t>test1</t>
@@ -65,10 +83,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -78,14 +96,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -98,8 +147,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -113,6 +163,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -127,47 +185,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -190,7 +209,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,31 +240,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,187 +255,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,11 +449,52 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -470,52 +529,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -536,145 +554,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1066,19 +1084,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="5"/>
   <cols>
     <col min="2" max="2" width="16.875" customWidth="1"/>
     <col min="3" max="3" width="18.25" customWidth="1"/>
+    <col min="4" max="4" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1091,41 +1110,59 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>0.13</v>
@@ -1133,13 +1170,19 @@
       <c r="D4" t="b">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>-127</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>3.1415926</v>
@@ -1147,14 +1190,25 @@
       <c r="D5" t="b">
         <v>0</v>
       </c>
+      <c r="E5">
+        <v>255</v>
+      </c>
+      <c r="F5">
+        <v>-129</v>
+      </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6"/>
       <c r="C6">
         <v>1234</v>
+      </c>
+      <c r="E6">
+        <v>256</v>
+      </c>
+      <c r="F6">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Refactoring] Refactor the type parse code.
</commit_message>
<xml_diff>
--- a/Files/Config/TestData.xlsx
+++ b/Files/Config/TestData.xlsx
@@ -83,10 +83,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -111,7 +111,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -134,9 +134,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -147,9 +147,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,32 +185,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -208,15 +208,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,9 +232,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -255,187 +255,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,71 +446,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -532,8 +467,62 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -546,6 +535,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -554,10 +554,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -575,7 +575,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -584,112 +584,112 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -1194,7 +1194,7 @@
         <v>255</v>
       </c>
       <c r="F5">
-        <v>-129</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">

</xml_diff>

<commit_message>
[Add Feature] Support edit list separator or Key/Value separator on GUI.
</commit_message>
<xml_diff>
--- a/Files/Config/TestData.xlsx
+++ b/Files/Config/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
   <si>
     <t>id</t>
   </si>
@@ -134,19 +134,26 @@
   </si>
   <si>
     <t>test string</t>
+  </si>
+  <si>
+    <t>dsaweq你好，笨蛋！@#￥%……&amp;*（）</t>
+  </si>
+  <si>
+    <t>!@#$%^&amp;*()_+QWERASDzxcv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -159,6 +166,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9.75"/>
+      <color rgb="FF2A2A2A"/>
+      <name val="Microsoft YaHei UI"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -173,11 +186,87 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -197,67 +286,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -273,38 +301,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,25 +332,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,151 +500,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,11 +526,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -526,32 +545,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -589,6 +582,26 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -596,16 +609,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -618,10 +631,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -630,137 +643,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -771,6 +784,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1160,7 +1179,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="20" customHeight="1" outlineLevelRow="5"/>
@@ -1293,7 +1312,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:9">
+    <row r="4" customHeight="1" spans="1:13">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1321,8 +1340,20 @@
       <c r="I4" s="3">
         <v>922337203685477</v>
       </c>
+      <c r="J4" s="4">
+        <v>3.45482148321398</v>
+      </c>
+      <c r="K4" s="1">
+        <v>10.0214510024561</v>
+      </c>
+      <c r="L4" s="5">
+        <v>9.99999999999999e+27</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="5" customHeight="1" spans="1:6">
+    <row r="5" customHeight="1" spans="1:13">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1337,6 +1368,18 @@
       </c>
       <c r="F5" s="1">
         <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>-3.45482148321398</v>
+      </c>
+      <c r="K5" s="1">
+        <v>-10.0214510024561</v>
+      </c>
+      <c r="L5" s="5">
+        <v>9.99999999999999e+27</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">

</xml_diff>

<commit_message>
[Add Feature] Add boolList and byteList type support.
</commit_message>
<xml_diff>
--- a/Files/Config/TestData.xlsx
+++ b/Files/Config/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
   <si>
     <t>id</t>
   </si>
@@ -57,6 +57,12 @@
     <t>testString</t>
   </si>
   <si>
+    <t>testBoolList</t>
+  </si>
+  <si>
+    <t>testByteList</t>
+  </si>
+  <si>
     <t>long</t>
   </si>
   <si>
@@ -94,6 +100,12 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>boolList</t>
+  </si>
+  <si>
+    <t>byteList</t>
   </si>
   <si>
     <t>ID</t>
@@ -136,7 +148,19 @@
     <t>test string</t>
   </si>
   <si>
-    <t>dsaweq你好，笨蛋！@#￥%……&amp;*（）</t>
+    <t>测试boolList</t>
+  </si>
+  <si>
+    <t>测试byteList</t>
+  </si>
+  <si>
+    <t>dsaweq你好！@#￥%……&amp;*（）</t>
+  </si>
+  <si>
+    <t>TRUE|false|0|1</t>
+  </si>
+  <si>
+    <t>0|1|-1|2|3|255</t>
   </si>
   <si>
     <t>!@#$%^&amp;*()_+QWERASDzxcv</t>
@@ -147,10 +171,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
   </numFmts>
   <fonts count="23">
@@ -173,6 +197,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -180,23 +242,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -223,63 +279,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,22 +304,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,6 +356,102 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -350,13 +470,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,151 +530,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,6 +547,50 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -537,15 +605,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,47 +641,12 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -631,10 +655,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -643,133 +667,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1176,10 +1200,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="20" customHeight="1" outlineLevelRow="5"/>
@@ -1189,7 +1213,7 @@
     <col min="10" max="16384" width="12.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:13">
+    <row r="1" customHeight="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1229,90 +1253,108 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" customHeight="1" spans="1:13">
+    <row r="2" customHeight="1" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:13">
+    <row r="3" customHeight="1" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:13">
+    <row r="4" customHeight="1" spans="1:15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1350,7 +1392,13 @@
         <v>9.99999999999999e+27</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:13">
@@ -1379,7 +1427,7 @@
         <v>9.99999999999999e+27</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">

</xml_diff>

<commit_message>
[Add Feature] Add more list type supports.
</commit_message>
<xml_diff>
--- a/Files/Config/TestData.xlsx
+++ b/Files/Config/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69">
   <si>
     <t>id</t>
   </si>
@@ -63,6 +63,21 @@
     <t>testByteList</t>
   </si>
   <si>
+    <t>testSByteList</t>
+  </si>
+  <si>
+    <t>testShortList</t>
+  </si>
+  <si>
+    <t>testUShortList</t>
+  </si>
+  <si>
+    <t>testIntList</t>
+  </si>
+  <si>
+    <t>testUIntList</t>
+  </si>
+  <si>
     <t>long</t>
   </si>
   <si>
@@ -106,6 +121,21 @@
   </si>
   <si>
     <t>byteList</t>
+  </si>
+  <si>
+    <t>sbyteList</t>
+  </si>
+  <si>
+    <t>shortList</t>
+  </si>
+  <si>
+    <t>ushortList</t>
+  </si>
+  <si>
+    <t>intList</t>
+  </si>
+  <si>
+    <t>uintList</t>
   </si>
   <si>
     <t>ID</t>
@@ -154,6 +184,21 @@
     <t>测试byteList</t>
   </si>
   <si>
+    <t>测试sbyteList</t>
+  </si>
+  <si>
+    <t>测试shortList</t>
+  </si>
+  <si>
+    <t>测试ushortList</t>
+  </si>
+  <si>
+    <t>测试intList</t>
+  </si>
+  <si>
+    <t>测试uintList</t>
+  </si>
+  <si>
     <t>dsaweq你好！@#￥%……&amp;*（）</t>
   </si>
   <si>
@@ -161,6 +206,21 @@
   </si>
   <si>
     <t>0|1|-1|2|3|255</t>
+  </si>
+  <si>
+    <t>123|43|-1|0</t>
+  </si>
+  <si>
+    <t>2|432|123|432</t>
+  </si>
+  <si>
+    <t>-1|2|4|0</t>
+  </si>
+  <si>
+    <t>1|2|3|34|</t>
+  </si>
+  <si>
+    <t>1|2|3</t>
   </si>
   <si>
     <t>!@#$%^&amp;*()_+QWERASDzxcv</t>
@@ -171,11 +231,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -203,6 +263,65 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -212,7 +331,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -220,7 +339,61 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,119 +406,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -356,187 +416,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,21 +607,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -574,22 +619,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,6 +644,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -624,17 +679,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,6 +696,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -655,10 +715,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -667,133 +727,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -815,6 +875,9 @@
     </xf>
     <xf numFmtId="7" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1200,10 +1263,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="20" customHeight="1" outlineLevelRow="5"/>
@@ -1213,7 +1276,7 @@
     <col min="10" max="16384" width="12.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:15">
+    <row r="1" customHeight="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1259,102 +1322,147 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" customHeight="1" spans="1:15">
+    <row r="2" customHeight="1" spans="1:20">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:15">
+    <row r="3" customHeight="1" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:15">
+    <row r="4" customHeight="1" spans="1:20">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1392,13 +1500,28 @@
         <v>9.99999999999999e+27</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:13">
@@ -1427,7 +1550,7 @@
         <v>9.99999999999999e+27</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">

</xml_diff>

<commit_message>
[Add Feature]Support all list type.
</commit_message>
<xml_diff>
--- a/Files/Config/TestData.xlsx
+++ b/Files/Config/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93">
   <si>
     <t>id</t>
   </si>
@@ -78,6 +78,24 @@
     <t>testUIntList</t>
   </si>
   <si>
+    <t>testLongList</t>
+  </si>
+  <si>
+    <t>testULongList</t>
+  </si>
+  <si>
+    <t>testFloatList</t>
+  </si>
+  <si>
+    <t>testDoubleList</t>
+  </si>
+  <si>
+    <t>testDecimalList</t>
+  </si>
+  <si>
+    <t>testStringList</t>
+  </si>
+  <si>
     <t>long</t>
   </si>
   <si>
@@ -136,6 +154,24 @@
   </si>
   <si>
     <t>uintList</t>
+  </si>
+  <si>
+    <t>longList</t>
+  </si>
+  <si>
+    <t>ulongList</t>
+  </si>
+  <si>
+    <t>floatList</t>
+  </si>
+  <si>
+    <t>doubleList</t>
+  </si>
+  <si>
+    <t>decimalList</t>
+  </si>
+  <si>
+    <t>stringList</t>
   </si>
   <si>
     <t>ID</t>
@@ -199,6 +235,24 @@
     <t>测试uintList</t>
   </si>
   <si>
+    <t>测试longList</t>
+  </si>
+  <si>
+    <t>测试ulongList</t>
+  </si>
+  <si>
+    <t>测试floatList</t>
+  </si>
+  <si>
+    <t>测试doubleList</t>
+  </si>
+  <si>
+    <t>测试decimalList</t>
+  </si>
+  <si>
+    <t>测试stringList</t>
+  </si>
+  <si>
     <t>dsaweq你好！@#￥%……&amp;*（）</t>
   </si>
   <si>
@@ -221,6 +275,42 @@
   </si>
   <si>
     <t>1|2|3</t>
+  </si>
+  <si>
+    <t>7|8|9|10</t>
+  </si>
+  <si>
+    <t>4|5|6|7</t>
+  </si>
+  <si>
+    <t>1.1|2.2|3.3|4.4</t>
+  </si>
+  <si>
+    <t>5.5|6.6|7.7|8.8</t>
+  </si>
+  <si>
+    <t>9.9999|10.11111|11.124454354|12.3</t>
+  </si>
+  <si>
+    <r>
+      <t>你好|hello|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="BatangChe"/>
+        <charset val="134"/>
+      </rPr>
+      <t>안녕하세요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
   <si>
     <t>!@#$%^&amp;*()_+QWERASDzxcv</t>
@@ -231,13 +321,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -257,6 +347,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -264,7 +361,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -292,6 +389,106 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -300,111 +497,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <sz val="12"/>
+      <name val="BatangChe"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -416,13 +511,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,19 +673,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,145 +691,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,16 +730,45 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -665,45 +789,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,10 +810,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -727,137 +822,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -875,6 +970,9 @@
     </xf>
     <xf numFmtId="7" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1263,20 +1361,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="20" customHeight="1" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="8" width="12.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="31.125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="12.625" style="1" customWidth="1"/>
+    <col min="10" max="21" width="12.625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.375" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="12.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:20">
+    <row r="1" customHeight="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1337,132 +1437,186 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" customHeight="1" spans="1:20">
+    <row r="2" customHeight="1" spans="1:26">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:20">
+    <row r="3" customHeight="1" spans="1:26">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:20">
+    <row r="4" customHeight="1" spans="1:26">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1500,28 +1654,46 @@
         <v>9.99999999999999e+27</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>65</v>
+        <v>82</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:13">
@@ -1550,7 +1722,7 @@
         <v>9.99999999999999e+27</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">

</xml_diff>

<commit_message>
[Fix Bug]Fix bug of ConfigEditor.
</commit_message>
<xml_diff>
--- a/Files/Config/TestData.xlsx
+++ b/Files/Config/TestData.xlsx
@@ -293,6 +293,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>你好|hello|</t>
     </r>
     <r>
@@ -321,11 +326,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -353,15 +358,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,7 +382,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -404,8 +411,16 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -426,6 +441,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,63 +495,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -511,13 +516,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,7 +672,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,157 +690,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,15 +707,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -729,6 +725,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -740,17 +760,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -773,6 +782,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -787,21 +807,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -810,10 +815,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -822,7 +827,7 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -831,124 +836,124 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1363,17 +1368,13 @@
   <sheetPr/>
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="20" customHeight="1" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="20" customHeight="1" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="8" width="12.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="31.125" style="1" customWidth="1"/>
-    <col min="10" max="21" width="12.625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="15.375" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="12.625" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="20.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:26">

</xml_diff>